<commit_message>
Finanl updates from simon
</commit_message>
<xml_diff>
--- a/Results/Farm_Data.xlsx
+++ b/Results/Farm_Data.xlsx
@@ -31,10 +31,10 @@
     <t>Field: E, Size sqm: 70, Type of grass: 3.</t>
   </si>
   <si>
-    <t>Field: Q, Size sqm: 70, Type of grass: 3.</t>
+    <t>Field: Q, Size sqm: 50, Type of grass: 1.</t>
   </si>
   <si>
-    <t>Field: W, Size sqm: 70, Type of grass: 3.</t>
+    <t>Field: W, Size sqm: 60, Type of grass: 2.</t>
   </si>
 </sst>
 </file>

</xml_diff>